<commit_message>
feat: LevelTable 연결 작업 및 기존 LevelData.Json 제거
  Assets/
  ├── Resources/
  │   ├── LevelData.json          ← (기존, 더 이상 사용 안 함)
  │   └── Tables/
  │       └── LevelTable.json     ← (새로 추가) Excel에서 생성
  ├── Scripts/
  │   ├── LevelManager.cs         ← (수정됨) LevelTable 사용
  │   └── Data/
  │       └── Generated/
  │           └── LevelTable.cs   ← (새로 추가) 테이블 관리 클래스
</commit_message>
<xml_diff>
--- a/wai_jigsaw/TableExporter/excel/data_stage.xlsx
+++ b/wai_jigsaw/TableExporter/excel/data_stage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DG-2507-PC-061\WAIDev\WAIDev\wai_jigsaw\TableExporter\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE93D4C-1B72-4ACD-B3B6-25E367470538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5439AD22-8B13-4CD9-A2B9-A25BBBD49973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="2505" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: LevelGroupTable 정보 추가
</commit_message>
<xml_diff>
--- a/wai_jigsaw/TableExporter/excel/data_stage.xlsx
+++ b/wai_jigsaw/TableExporter/excel/data_stage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DG-2507-PC-061\WAIDev\WAIDev\wai_jigsaw\TableExporter\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90858426-36C9-43FC-A874-6EBDDB0FF34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046596A5-24F5-4AFF-AB36-006A279A6B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1710" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Level" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="59">
   <si>
     <t>data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -210,6 +210,54 @@
   </si>
   <si>
     <t>Name2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Reward_Group03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Reward_Group04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Reward_Group05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Reward_Group06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Reward_Group07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Reward_Group08</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -615,10 +663,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:H54"/>
+  <dimension ref="A2:H204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -802,13 +850,13 @@
         <v>18</v>
       </c>
       <c r="D9" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="6">
         <v>10</v>
@@ -1268,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G29" s="6">
         <v>10</v>
@@ -1849,6 +1897,3456 @@
         <v>10</v>
       </c>
       <c r="H54" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="5">
+        <v>51</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="6">
+        <v>3</v>
+      </c>
+      <c r="E55" s="6">
+        <v>3</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G55" s="6">
+        <v>10</v>
+      </c>
+      <c r="H55" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="5">
+        <v>52</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="6">
+        <v>3</v>
+      </c>
+      <c r="E56" s="6">
+        <v>3</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="6">
+        <v>10</v>
+      </c>
+      <c r="H56" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="5">
+        <v>53</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="6">
+        <v>3</v>
+      </c>
+      <c r="E57" s="6">
+        <v>3</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G57" s="6">
+        <v>10</v>
+      </c>
+      <c r="H57" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="5">
+        <v>54</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="6">
+        <v>3</v>
+      </c>
+      <c r="E58" s="6">
+        <v>3</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G58" s="6">
+        <v>10</v>
+      </c>
+      <c r="H58" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="5">
+        <v>55</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="6">
+        <v>3</v>
+      </c>
+      <c r="E59" s="6">
+        <v>3</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G59" s="6">
+        <v>10</v>
+      </c>
+      <c r="H59" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="5">
+        <v>56</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="6">
+        <v>3</v>
+      </c>
+      <c r="E60" s="6">
+        <v>3</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="6">
+        <v>10</v>
+      </c>
+      <c r="H60" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="5">
+        <v>57</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="6">
+        <v>3</v>
+      </c>
+      <c r="E61" s="6">
+        <v>3</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G61" s="6">
+        <v>10</v>
+      </c>
+      <c r="H61" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="5">
+        <v>58</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="6">
+        <v>3</v>
+      </c>
+      <c r="E62" s="6">
+        <v>3</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G62" s="6">
+        <v>10</v>
+      </c>
+      <c r="H62" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="5">
+        <v>59</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="6">
+        <v>3</v>
+      </c>
+      <c r="E63" s="6">
+        <v>3</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G63" s="6">
+        <v>10</v>
+      </c>
+      <c r="H63" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="5">
+        <v>60</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="6">
+        <v>3</v>
+      </c>
+      <c r="E64" s="6">
+        <v>3</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="6">
+        <v>10</v>
+      </c>
+      <c r="H64" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="5">
+        <v>61</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="6">
+        <v>3</v>
+      </c>
+      <c r="E65" s="6">
+        <v>3</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G65" s="6">
+        <v>10</v>
+      </c>
+      <c r="H65" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="5">
+        <v>62</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="6">
+        <v>3</v>
+      </c>
+      <c r="E66" s="6">
+        <v>3</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G66" s="6">
+        <v>10</v>
+      </c>
+      <c r="H66" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="5">
+        <v>63</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="6">
+        <v>3</v>
+      </c>
+      <c r="E67" s="6">
+        <v>3</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G67" s="6">
+        <v>10</v>
+      </c>
+      <c r="H67" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="5">
+        <v>64</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="6">
+        <v>3</v>
+      </c>
+      <c r="E68" s="6">
+        <v>3</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G68" s="6">
+        <v>10</v>
+      </c>
+      <c r="H68" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="5">
+        <v>65</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="6">
+        <v>3</v>
+      </c>
+      <c r="E69" s="6">
+        <v>3</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G69" s="6">
+        <v>10</v>
+      </c>
+      <c r="H69" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="5">
+        <v>66</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="6">
+        <v>3</v>
+      </c>
+      <c r="E70" s="6">
+        <v>3</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G70" s="6">
+        <v>10</v>
+      </c>
+      <c r="H70" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="5">
+        <v>67</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="6">
+        <v>3</v>
+      </c>
+      <c r="E71" s="6">
+        <v>3</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G71" s="6">
+        <v>10</v>
+      </c>
+      <c r="H71" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="5">
+        <v>68</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="6">
+        <v>3</v>
+      </c>
+      <c r="E72" s="6">
+        <v>3</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G72" s="6">
+        <v>10</v>
+      </c>
+      <c r="H72" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="5">
+        <v>69</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="6">
+        <v>3</v>
+      </c>
+      <c r="E73" s="6">
+        <v>3</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G73" s="6">
+        <v>10</v>
+      </c>
+      <c r="H73" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="5">
+        <v>70</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="6">
+        <v>3</v>
+      </c>
+      <c r="E74" s="6">
+        <v>3</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G74" s="6">
+        <v>10</v>
+      </c>
+      <c r="H74" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="5">
+        <v>71</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="6">
+        <v>3</v>
+      </c>
+      <c r="E75" s="6">
+        <v>3</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G75" s="6">
+        <v>10</v>
+      </c>
+      <c r="H75" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="5">
+        <v>72</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" s="6">
+        <v>3</v>
+      </c>
+      <c r="E76" s="6">
+        <v>3</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G76" s="6">
+        <v>10</v>
+      </c>
+      <c r="H76" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="5">
+        <v>73</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="6">
+        <v>3</v>
+      </c>
+      <c r="E77" s="6">
+        <v>3</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G77" s="6">
+        <v>10</v>
+      </c>
+      <c r="H77" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="5">
+        <v>74</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" s="6">
+        <v>3</v>
+      </c>
+      <c r="E78" s="6">
+        <v>3</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G78" s="6">
+        <v>10</v>
+      </c>
+      <c r="H78" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="5">
+        <v>75</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="6">
+        <v>3</v>
+      </c>
+      <c r="E79" s="6">
+        <v>3</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G79" s="6">
+        <v>10</v>
+      </c>
+      <c r="H79" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="5">
+        <v>76</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" s="6">
+        <v>3</v>
+      </c>
+      <c r="E80" s="6">
+        <v>3</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G80" s="6">
+        <v>10</v>
+      </c>
+      <c r="H80" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="5">
+        <v>77</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" s="6">
+        <v>3</v>
+      </c>
+      <c r="E81" s="6">
+        <v>3</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G81" s="6">
+        <v>10</v>
+      </c>
+      <c r="H81" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="5">
+        <v>78</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="6">
+        <v>3</v>
+      </c>
+      <c r="E82" s="6">
+        <v>3</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G82" s="6">
+        <v>10</v>
+      </c>
+      <c r="H82" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="5">
+        <v>79</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" s="6">
+        <v>3</v>
+      </c>
+      <c r="E83" s="6">
+        <v>3</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G83" s="6">
+        <v>10</v>
+      </c>
+      <c r="H83" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="5">
+        <v>80</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" s="6">
+        <v>3</v>
+      </c>
+      <c r="E84" s="6">
+        <v>3</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G84" s="6">
+        <v>10</v>
+      </c>
+      <c r="H84" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="5">
+        <v>81</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" s="6">
+        <v>3</v>
+      </c>
+      <c r="E85" s="6">
+        <v>3</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G85" s="6">
+        <v>10</v>
+      </c>
+      <c r="H85" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="5">
+        <v>82</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" s="6">
+        <v>3</v>
+      </c>
+      <c r="E86" s="6">
+        <v>3</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G86" s="6">
+        <v>10</v>
+      </c>
+      <c r="H86" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="5">
+        <v>83</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" s="6">
+        <v>3</v>
+      </c>
+      <c r="E87" s="6">
+        <v>3</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G87" s="6">
+        <v>10</v>
+      </c>
+      <c r="H87" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="5">
+        <v>84</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" s="6">
+        <v>3</v>
+      </c>
+      <c r="E88" s="6">
+        <v>3</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G88" s="6">
+        <v>10</v>
+      </c>
+      <c r="H88" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="5">
+        <v>85</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="6">
+        <v>3</v>
+      </c>
+      <c r="E89" s="6">
+        <v>3</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G89" s="6">
+        <v>10</v>
+      </c>
+      <c r="H89" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="5">
+        <v>86</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" s="6">
+        <v>3</v>
+      </c>
+      <c r="E90" s="6">
+        <v>3</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G90" s="6">
+        <v>10</v>
+      </c>
+      <c r="H90" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="5">
+        <v>87</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="6">
+        <v>3</v>
+      </c>
+      <c r="E91" s="6">
+        <v>3</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G91" s="6">
+        <v>10</v>
+      </c>
+      <c r="H91" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="5">
+        <v>88</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" s="6">
+        <v>3</v>
+      </c>
+      <c r="E92" s="6">
+        <v>3</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G92" s="6">
+        <v>10</v>
+      </c>
+      <c r="H92" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="5">
+        <v>89</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" s="6">
+        <v>3</v>
+      </c>
+      <c r="E93" s="6">
+        <v>3</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G93" s="6">
+        <v>10</v>
+      </c>
+      <c r="H93" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="5">
+        <v>90</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" s="6">
+        <v>3</v>
+      </c>
+      <c r="E94" s="6">
+        <v>3</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G94" s="6">
+        <v>10</v>
+      </c>
+      <c r="H94" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="5">
+        <v>91</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" s="6">
+        <v>3</v>
+      </c>
+      <c r="E95" s="6">
+        <v>3</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G95" s="6">
+        <v>10</v>
+      </c>
+      <c r="H95" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="5">
+        <v>92</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" s="6">
+        <v>3</v>
+      </c>
+      <c r="E96" s="6">
+        <v>3</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G96" s="6">
+        <v>10</v>
+      </c>
+      <c r="H96" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="5">
+        <v>93</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" s="6">
+        <v>3</v>
+      </c>
+      <c r="E97" s="6">
+        <v>3</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G97" s="6">
+        <v>10</v>
+      </c>
+      <c r="H97" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="5">
+        <v>94</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" s="6">
+        <v>3</v>
+      </c>
+      <c r="E98" s="6">
+        <v>3</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G98" s="6">
+        <v>10</v>
+      </c>
+      <c r="H98" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="5">
+        <v>95</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" s="6">
+        <v>3</v>
+      </c>
+      <c r="E99" s="6">
+        <v>3</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G99" s="6">
+        <v>10</v>
+      </c>
+      <c r="H99" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="5">
+        <v>96</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" s="6">
+        <v>3</v>
+      </c>
+      <c r="E100" s="6">
+        <v>3</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G100" s="6">
+        <v>10</v>
+      </c>
+      <c r="H100" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="5">
+        <v>97</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" s="6">
+        <v>3</v>
+      </c>
+      <c r="E101" s="6">
+        <v>3</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G101" s="6">
+        <v>10</v>
+      </c>
+      <c r="H101" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="5">
+        <v>98</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" s="6">
+        <v>3</v>
+      </c>
+      <c r="E102" s="6">
+        <v>3</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G102" s="6">
+        <v>10</v>
+      </c>
+      <c r="H102" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="5">
+        <v>99</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D103" s="6">
+        <v>3</v>
+      </c>
+      <c r="E103" s="6">
+        <v>3</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G103" s="6">
+        <v>10</v>
+      </c>
+      <c r="H103" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="5">
+        <v>100</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" s="6">
+        <v>3</v>
+      </c>
+      <c r="E104" s="6">
+        <v>3</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G104" s="6">
+        <v>10</v>
+      </c>
+      <c r="H104" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="5">
+        <v>101</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" s="6">
+        <v>3</v>
+      </c>
+      <c r="E105" s="6">
+        <v>3</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G105" s="6">
+        <v>10</v>
+      </c>
+      <c r="H105" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="5">
+        <v>102</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" s="6">
+        <v>3</v>
+      </c>
+      <c r="E106" s="6">
+        <v>3</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G106" s="6">
+        <v>10</v>
+      </c>
+      <c r="H106" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="5">
+        <v>103</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107" s="6">
+        <v>3</v>
+      </c>
+      <c r="E107" s="6">
+        <v>3</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G107" s="6">
+        <v>10</v>
+      </c>
+      <c r="H107" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="5">
+        <v>104</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" s="6">
+        <v>3</v>
+      </c>
+      <c r="E108" s="6">
+        <v>3</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G108" s="6">
+        <v>10</v>
+      </c>
+      <c r="H108" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="5">
+        <v>105</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" s="6">
+        <v>3</v>
+      </c>
+      <c r="E109" s="6">
+        <v>3</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G109" s="6">
+        <v>10</v>
+      </c>
+      <c r="H109" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="5">
+        <v>106</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" s="6">
+        <v>3</v>
+      </c>
+      <c r="E110" s="6">
+        <v>3</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G110" s="6">
+        <v>10</v>
+      </c>
+      <c r="H110" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B111" s="5">
+        <v>107</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D111" s="6">
+        <v>3</v>
+      </c>
+      <c r="E111" s="6">
+        <v>3</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G111" s="6">
+        <v>10</v>
+      </c>
+      <c r="H111" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="5">
+        <v>108</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" s="6">
+        <v>3</v>
+      </c>
+      <c r="E112" s="6">
+        <v>3</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G112" s="6">
+        <v>10</v>
+      </c>
+      <c r="H112" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" s="5">
+        <v>109</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D113" s="6">
+        <v>3</v>
+      </c>
+      <c r="E113" s="6">
+        <v>3</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G113" s="6">
+        <v>10</v>
+      </c>
+      <c r="H113" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B114" s="5">
+        <v>110</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" s="6">
+        <v>3</v>
+      </c>
+      <c r="E114" s="6">
+        <v>3</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G114" s="6">
+        <v>10</v>
+      </c>
+      <c r="H114" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115" s="5">
+        <v>111</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" s="6">
+        <v>3</v>
+      </c>
+      <c r="E115" s="6">
+        <v>3</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G115" s="6">
+        <v>10</v>
+      </c>
+      <c r="H115" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116" s="5">
+        <v>112</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" s="6">
+        <v>3</v>
+      </c>
+      <c r="E116" s="6">
+        <v>3</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G116" s="6">
+        <v>10</v>
+      </c>
+      <c r="H116" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B117" s="5">
+        <v>113</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117" s="6">
+        <v>3</v>
+      </c>
+      <c r="E117" s="6">
+        <v>3</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G117" s="6">
+        <v>10</v>
+      </c>
+      <c r="H117" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" s="5">
+        <v>114</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" s="6">
+        <v>3</v>
+      </c>
+      <c r="E118" s="6">
+        <v>3</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G118" s="6">
+        <v>10</v>
+      </c>
+      <c r="H118" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B119" s="5">
+        <v>115</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" s="6">
+        <v>3</v>
+      </c>
+      <c r="E119" s="6">
+        <v>3</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G119" s="6">
+        <v>10</v>
+      </c>
+      <c r="H119" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B120" s="5">
+        <v>116</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" s="6">
+        <v>3</v>
+      </c>
+      <c r="E120" s="6">
+        <v>3</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G120" s="6">
+        <v>10</v>
+      </c>
+      <c r="H120" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B121" s="5">
+        <v>117</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D121" s="6">
+        <v>3</v>
+      </c>
+      <c r="E121" s="6">
+        <v>3</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G121" s="6">
+        <v>10</v>
+      </c>
+      <c r="H121" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="5">
+        <v>118</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" s="6">
+        <v>3</v>
+      </c>
+      <c r="E122" s="6">
+        <v>3</v>
+      </c>
+      <c r="F122" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G122" s="6">
+        <v>10</v>
+      </c>
+      <c r="H122" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B123" s="5">
+        <v>119</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" s="6">
+        <v>3</v>
+      </c>
+      <c r="E123" s="6">
+        <v>3</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G123" s="6">
+        <v>10</v>
+      </c>
+      <c r="H123" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124" s="5">
+        <v>120</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" s="6">
+        <v>3</v>
+      </c>
+      <c r="E124" s="6">
+        <v>3</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G124" s="6">
+        <v>10</v>
+      </c>
+      <c r="H124" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B125" s="5">
+        <v>121</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" s="6">
+        <v>3</v>
+      </c>
+      <c r="E125" s="6">
+        <v>3</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G125" s="6">
+        <v>10</v>
+      </c>
+      <c r="H125" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="5">
+        <v>122</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D126" s="6">
+        <v>3</v>
+      </c>
+      <c r="E126" s="6">
+        <v>3</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G126" s="6">
+        <v>10</v>
+      </c>
+      <c r="H126" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="5">
+        <v>123</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D127" s="6">
+        <v>3</v>
+      </c>
+      <c r="E127" s="6">
+        <v>3</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G127" s="6">
+        <v>10</v>
+      </c>
+      <c r="H127" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="5">
+        <v>124</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D128" s="6">
+        <v>3</v>
+      </c>
+      <c r="E128" s="6">
+        <v>3</v>
+      </c>
+      <c r="F128" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G128" s="6">
+        <v>10</v>
+      </c>
+      <c r="H128" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="5">
+        <v>125</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D129" s="6">
+        <v>3</v>
+      </c>
+      <c r="E129" s="6">
+        <v>3</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G129" s="6">
+        <v>10</v>
+      </c>
+      <c r="H129" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="5">
+        <v>126</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D130" s="6">
+        <v>3</v>
+      </c>
+      <c r="E130" s="6">
+        <v>3</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G130" s="6">
+        <v>10</v>
+      </c>
+      <c r="H130" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="5">
+        <v>127</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D131" s="6">
+        <v>3</v>
+      </c>
+      <c r="E131" s="6">
+        <v>3</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G131" s="6">
+        <v>10</v>
+      </c>
+      <c r="H131" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="5">
+        <v>128</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" s="6">
+        <v>3</v>
+      </c>
+      <c r="E132" s="6">
+        <v>3</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G132" s="6">
+        <v>10</v>
+      </c>
+      <c r="H132" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="5">
+        <v>129</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D133" s="6">
+        <v>3</v>
+      </c>
+      <c r="E133" s="6">
+        <v>3</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G133" s="6">
+        <v>10</v>
+      </c>
+      <c r="H133" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="5">
+        <v>130</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D134" s="6">
+        <v>3</v>
+      </c>
+      <c r="E134" s="6">
+        <v>3</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G134" s="6">
+        <v>10</v>
+      </c>
+      <c r="H134" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="5">
+        <v>131</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D135" s="6">
+        <v>3</v>
+      </c>
+      <c r="E135" s="6">
+        <v>3</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G135" s="6">
+        <v>10</v>
+      </c>
+      <c r="H135" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="5">
+        <v>132</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" s="6">
+        <v>3</v>
+      </c>
+      <c r="E136" s="6">
+        <v>3</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G136" s="6">
+        <v>10</v>
+      </c>
+      <c r="H136" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="5">
+        <v>133</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D137" s="6">
+        <v>3</v>
+      </c>
+      <c r="E137" s="6">
+        <v>3</v>
+      </c>
+      <c r="F137" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G137" s="6">
+        <v>10</v>
+      </c>
+      <c r="H137" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="5">
+        <v>134</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D138" s="6">
+        <v>3</v>
+      </c>
+      <c r="E138" s="6">
+        <v>3</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G138" s="6">
+        <v>10</v>
+      </c>
+      <c r="H138" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="5">
+        <v>135</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D139" s="6">
+        <v>3</v>
+      </c>
+      <c r="E139" s="6">
+        <v>3</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G139" s="6">
+        <v>10</v>
+      </c>
+      <c r="H139" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="5">
+        <v>136</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D140" s="6">
+        <v>3</v>
+      </c>
+      <c r="E140" s="6">
+        <v>3</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G140" s="6">
+        <v>10</v>
+      </c>
+      <c r="H140" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="5">
+        <v>137</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D141" s="6">
+        <v>3</v>
+      </c>
+      <c r="E141" s="6">
+        <v>3</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G141" s="6">
+        <v>10</v>
+      </c>
+      <c r="H141" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="5">
+        <v>138</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" s="6">
+        <v>3</v>
+      </c>
+      <c r="E142" s="6">
+        <v>3</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G142" s="6">
+        <v>10</v>
+      </c>
+      <c r="H142" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="5">
+        <v>139</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" s="6">
+        <v>3</v>
+      </c>
+      <c r="E143" s="6">
+        <v>3</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G143" s="6">
+        <v>10</v>
+      </c>
+      <c r="H143" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B144" s="5">
+        <v>140</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D144" s="6">
+        <v>3</v>
+      </c>
+      <c r="E144" s="6">
+        <v>3</v>
+      </c>
+      <c r="F144" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G144" s="6">
+        <v>10</v>
+      </c>
+      <c r="H144" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B145" s="5">
+        <v>141</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D145" s="6">
+        <v>3</v>
+      </c>
+      <c r="E145" s="6">
+        <v>3</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G145" s="6">
+        <v>10</v>
+      </c>
+      <c r="H145" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B146" s="5">
+        <v>142</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D146" s="6">
+        <v>3</v>
+      </c>
+      <c r="E146" s="6">
+        <v>3</v>
+      </c>
+      <c r="F146" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G146" s="6">
+        <v>10</v>
+      </c>
+      <c r="H146" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B147" s="5">
+        <v>143</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D147" s="6">
+        <v>3</v>
+      </c>
+      <c r="E147" s="6">
+        <v>3</v>
+      </c>
+      <c r="F147" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G147" s="6">
+        <v>10</v>
+      </c>
+      <c r="H147" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B148" s="5">
+        <v>144</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D148" s="6">
+        <v>3</v>
+      </c>
+      <c r="E148" s="6">
+        <v>3</v>
+      </c>
+      <c r="F148" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G148" s="6">
+        <v>10</v>
+      </c>
+      <c r="H148" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B149" s="5">
+        <v>145</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D149" s="6">
+        <v>3</v>
+      </c>
+      <c r="E149" s="6">
+        <v>3</v>
+      </c>
+      <c r="F149" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G149" s="6">
+        <v>10</v>
+      </c>
+      <c r="H149" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B150" s="5">
+        <v>146</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D150" s="6">
+        <v>3</v>
+      </c>
+      <c r="E150" s="6">
+        <v>3</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G150" s="6">
+        <v>10</v>
+      </c>
+      <c r="H150" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B151" s="5">
+        <v>147</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D151" s="6">
+        <v>3</v>
+      </c>
+      <c r="E151" s="6">
+        <v>3</v>
+      </c>
+      <c r="F151" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G151" s="6">
+        <v>10</v>
+      </c>
+      <c r="H151" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B152" s="5">
+        <v>148</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D152" s="6">
+        <v>3</v>
+      </c>
+      <c r="E152" s="6">
+        <v>3</v>
+      </c>
+      <c r="F152" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G152" s="6">
+        <v>10</v>
+      </c>
+      <c r="H152" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B153" s="5">
+        <v>149</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D153" s="6">
+        <v>3</v>
+      </c>
+      <c r="E153" s="6">
+        <v>3</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G153" s="6">
+        <v>10</v>
+      </c>
+      <c r="H153" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B154" s="5">
+        <v>150</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D154" s="6">
+        <v>3</v>
+      </c>
+      <c r="E154" s="6">
+        <v>3</v>
+      </c>
+      <c r="F154" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G154" s="6">
+        <v>10</v>
+      </c>
+      <c r="H154" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B155" s="5">
+        <v>151</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D155" s="6">
+        <v>3</v>
+      </c>
+      <c r="E155" s="6">
+        <v>3</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G155" s="6">
+        <v>10</v>
+      </c>
+      <c r="H155" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B156" s="5">
+        <v>152</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D156" s="6">
+        <v>3</v>
+      </c>
+      <c r="E156" s="6">
+        <v>3</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G156" s="6">
+        <v>10</v>
+      </c>
+      <c r="H156" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B157" s="5">
+        <v>153</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D157" s="6">
+        <v>3</v>
+      </c>
+      <c r="E157" s="6">
+        <v>3</v>
+      </c>
+      <c r="F157" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G157" s="6">
+        <v>10</v>
+      </c>
+      <c r="H157" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B158" s="5">
+        <v>154</v>
+      </c>
+      <c r="C158" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D158" s="6">
+        <v>3</v>
+      </c>
+      <c r="E158" s="6">
+        <v>3</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G158" s="6">
+        <v>10</v>
+      </c>
+      <c r="H158" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B159" s="5">
+        <v>155</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D159" s="6">
+        <v>3</v>
+      </c>
+      <c r="E159" s="6">
+        <v>3</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G159" s="6">
+        <v>10</v>
+      </c>
+      <c r="H159" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B160" s="5">
+        <v>156</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D160" s="6">
+        <v>3</v>
+      </c>
+      <c r="E160" s="6">
+        <v>3</v>
+      </c>
+      <c r="F160" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G160" s="6">
+        <v>10</v>
+      </c>
+      <c r="H160" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B161" s="5">
+        <v>157</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D161" s="6">
+        <v>3</v>
+      </c>
+      <c r="E161" s="6">
+        <v>3</v>
+      </c>
+      <c r="F161" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G161" s="6">
+        <v>10</v>
+      </c>
+      <c r="H161" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B162" s="5">
+        <v>158</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D162" s="6">
+        <v>3</v>
+      </c>
+      <c r="E162" s="6">
+        <v>3</v>
+      </c>
+      <c r="F162" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G162" s="6">
+        <v>10</v>
+      </c>
+      <c r="H162" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B163" s="5">
+        <v>159</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D163" s="6">
+        <v>3</v>
+      </c>
+      <c r="E163" s="6">
+        <v>3</v>
+      </c>
+      <c r="F163" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G163" s="6">
+        <v>10</v>
+      </c>
+      <c r="H163" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B164" s="5">
+        <v>160</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D164" s="6">
+        <v>3</v>
+      </c>
+      <c r="E164" s="6">
+        <v>3</v>
+      </c>
+      <c r="F164" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G164" s="6">
+        <v>10</v>
+      </c>
+      <c r="H164" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B165" s="5">
+        <v>161</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D165" s="6">
+        <v>3</v>
+      </c>
+      <c r="E165" s="6">
+        <v>3</v>
+      </c>
+      <c r="F165" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G165" s="6">
+        <v>10</v>
+      </c>
+      <c r="H165" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B166" s="5">
+        <v>162</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D166" s="6">
+        <v>3</v>
+      </c>
+      <c r="E166" s="6">
+        <v>3</v>
+      </c>
+      <c r="F166" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G166" s="6">
+        <v>10</v>
+      </c>
+      <c r="H166" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B167" s="5">
+        <v>163</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D167" s="6">
+        <v>3</v>
+      </c>
+      <c r="E167" s="6">
+        <v>3</v>
+      </c>
+      <c r="F167" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G167" s="6">
+        <v>10</v>
+      </c>
+      <c r="H167" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B168" s="5">
+        <v>164</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D168" s="6">
+        <v>3</v>
+      </c>
+      <c r="E168" s="6">
+        <v>3</v>
+      </c>
+      <c r="F168" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G168" s="6">
+        <v>10</v>
+      </c>
+      <c r="H168" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B169" s="5">
+        <v>165</v>
+      </c>
+      <c r="C169" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D169" s="6">
+        <v>3</v>
+      </c>
+      <c r="E169" s="6">
+        <v>3</v>
+      </c>
+      <c r="F169" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G169" s="6">
+        <v>10</v>
+      </c>
+      <c r="H169" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B170" s="5">
+        <v>166</v>
+      </c>
+      <c r="C170" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D170" s="6">
+        <v>3</v>
+      </c>
+      <c r="E170" s="6">
+        <v>3</v>
+      </c>
+      <c r="F170" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G170" s="6">
+        <v>10</v>
+      </c>
+      <c r="H170" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B171" s="5">
+        <v>167</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D171" s="6">
+        <v>3</v>
+      </c>
+      <c r="E171" s="6">
+        <v>3</v>
+      </c>
+      <c r="F171" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G171" s="6">
+        <v>10</v>
+      </c>
+      <c r="H171" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B172" s="5">
+        <v>168</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D172" s="6">
+        <v>3</v>
+      </c>
+      <c r="E172" s="6">
+        <v>3</v>
+      </c>
+      <c r="F172" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G172" s="6">
+        <v>10</v>
+      </c>
+      <c r="H172" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B173" s="5">
+        <v>169</v>
+      </c>
+      <c r="C173" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D173" s="6">
+        <v>3</v>
+      </c>
+      <c r="E173" s="6">
+        <v>3</v>
+      </c>
+      <c r="F173" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G173" s="6">
+        <v>10</v>
+      </c>
+      <c r="H173" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B174" s="5">
+        <v>170</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D174" s="6">
+        <v>3</v>
+      </c>
+      <c r="E174" s="6">
+        <v>3</v>
+      </c>
+      <c r="F174" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G174" s="6">
+        <v>10</v>
+      </c>
+      <c r="H174" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B175" s="5">
+        <v>171</v>
+      </c>
+      <c r="C175" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D175" s="6">
+        <v>3</v>
+      </c>
+      <c r="E175" s="6">
+        <v>3</v>
+      </c>
+      <c r="F175" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G175" s="6">
+        <v>10</v>
+      </c>
+      <c r="H175" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B176" s="5">
+        <v>172</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D176" s="6">
+        <v>3</v>
+      </c>
+      <c r="E176" s="6">
+        <v>3</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G176" s="6">
+        <v>10</v>
+      </c>
+      <c r="H176" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B177" s="5">
+        <v>173</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D177" s="6">
+        <v>3</v>
+      </c>
+      <c r="E177" s="6">
+        <v>3</v>
+      </c>
+      <c r="F177" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G177" s="6">
+        <v>10</v>
+      </c>
+      <c r="H177" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B178" s="5">
+        <v>174</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D178" s="6">
+        <v>3</v>
+      </c>
+      <c r="E178" s="6">
+        <v>3</v>
+      </c>
+      <c r="F178" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G178" s="6">
+        <v>10</v>
+      </c>
+      <c r="H178" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B179" s="5">
+        <v>175</v>
+      </c>
+      <c r="C179" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D179" s="6">
+        <v>3</v>
+      </c>
+      <c r="E179" s="6">
+        <v>3</v>
+      </c>
+      <c r="F179" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G179" s="6">
+        <v>10</v>
+      </c>
+      <c r="H179" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B180" s="5">
+        <v>176</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D180" s="6">
+        <v>3</v>
+      </c>
+      <c r="E180" s="6">
+        <v>3</v>
+      </c>
+      <c r="F180" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G180" s="6">
+        <v>10</v>
+      </c>
+      <c r="H180" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B181" s="5">
+        <v>177</v>
+      </c>
+      <c r="C181" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D181" s="6">
+        <v>3</v>
+      </c>
+      <c r="E181" s="6">
+        <v>3</v>
+      </c>
+      <c r="F181" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G181" s="6">
+        <v>10</v>
+      </c>
+      <c r="H181" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B182" s="5">
+        <v>178</v>
+      </c>
+      <c r="C182" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D182" s="6">
+        <v>3</v>
+      </c>
+      <c r="E182" s="6">
+        <v>3</v>
+      </c>
+      <c r="F182" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G182" s="6">
+        <v>10</v>
+      </c>
+      <c r="H182" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B183" s="5">
+        <v>179</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D183" s="6">
+        <v>3</v>
+      </c>
+      <c r="E183" s="6">
+        <v>3</v>
+      </c>
+      <c r="F183" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G183" s="6">
+        <v>10</v>
+      </c>
+      <c r="H183" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B184" s="5">
+        <v>180</v>
+      </c>
+      <c r="C184" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D184" s="6">
+        <v>3</v>
+      </c>
+      <c r="E184" s="6">
+        <v>3</v>
+      </c>
+      <c r="F184" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G184" s="6">
+        <v>10</v>
+      </c>
+      <c r="H184" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B185" s="5">
+        <v>181</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D185" s="6">
+        <v>3</v>
+      </c>
+      <c r="E185" s="6">
+        <v>3</v>
+      </c>
+      <c r="F185" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G185" s="6">
+        <v>10</v>
+      </c>
+      <c r="H185" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B186" s="5">
+        <v>182</v>
+      </c>
+      <c r="C186" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D186" s="6">
+        <v>3</v>
+      </c>
+      <c r="E186" s="6">
+        <v>3</v>
+      </c>
+      <c r="F186" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G186" s="6">
+        <v>10</v>
+      </c>
+      <c r="H186" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B187" s="5">
+        <v>183</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D187" s="6">
+        <v>3</v>
+      </c>
+      <c r="E187" s="6">
+        <v>3</v>
+      </c>
+      <c r="F187" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G187" s="6">
+        <v>10</v>
+      </c>
+      <c r="H187" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B188" s="5">
+        <v>184</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D188" s="6">
+        <v>3</v>
+      </c>
+      <c r="E188" s="6">
+        <v>3</v>
+      </c>
+      <c r="F188" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G188" s="6">
+        <v>10</v>
+      </c>
+      <c r="H188" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B189" s="5">
+        <v>185</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D189" s="6">
+        <v>3</v>
+      </c>
+      <c r="E189" s="6">
+        <v>3</v>
+      </c>
+      <c r="F189" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G189" s="6">
+        <v>10</v>
+      </c>
+      <c r="H189" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B190" s="5">
+        <v>186</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D190" s="6">
+        <v>3</v>
+      </c>
+      <c r="E190" s="6">
+        <v>3</v>
+      </c>
+      <c r="F190" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G190" s="6">
+        <v>10</v>
+      </c>
+      <c r="H190" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B191" s="5">
+        <v>187</v>
+      </c>
+      <c r="C191" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D191" s="6">
+        <v>3</v>
+      </c>
+      <c r="E191" s="6">
+        <v>3</v>
+      </c>
+      <c r="F191" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G191" s="6">
+        <v>10</v>
+      </c>
+      <c r="H191" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="192" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B192" s="5">
+        <v>188</v>
+      </c>
+      <c r="C192" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D192" s="6">
+        <v>3</v>
+      </c>
+      <c r="E192" s="6">
+        <v>3</v>
+      </c>
+      <c r="F192" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G192" s="6">
+        <v>10</v>
+      </c>
+      <c r="H192" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B193" s="5">
+        <v>189</v>
+      </c>
+      <c r="C193" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D193" s="6">
+        <v>3</v>
+      </c>
+      <c r="E193" s="6">
+        <v>3</v>
+      </c>
+      <c r="F193" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G193" s="6">
+        <v>10</v>
+      </c>
+      <c r="H193" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B194" s="5">
+        <v>190</v>
+      </c>
+      <c r="C194" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D194" s="6">
+        <v>3</v>
+      </c>
+      <c r="E194" s="6">
+        <v>3</v>
+      </c>
+      <c r="F194" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G194" s="6">
+        <v>10</v>
+      </c>
+      <c r="H194" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B195" s="5">
+        <v>191</v>
+      </c>
+      <c r="C195" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D195" s="6">
+        <v>3</v>
+      </c>
+      <c r="E195" s="6">
+        <v>3</v>
+      </c>
+      <c r="F195" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G195" s="6">
+        <v>10</v>
+      </c>
+      <c r="H195" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="196" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B196" s="5">
+        <v>192</v>
+      </c>
+      <c r="C196" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D196" s="6">
+        <v>3</v>
+      </c>
+      <c r="E196" s="6">
+        <v>3</v>
+      </c>
+      <c r="F196" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G196" s="6">
+        <v>10</v>
+      </c>
+      <c r="H196" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="197" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B197" s="5">
+        <v>193</v>
+      </c>
+      <c r="C197" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D197" s="6">
+        <v>3</v>
+      </c>
+      <c r="E197" s="6">
+        <v>3</v>
+      </c>
+      <c r="F197" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G197" s="6">
+        <v>10</v>
+      </c>
+      <c r="H197" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="198" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B198" s="5">
+        <v>194</v>
+      </c>
+      <c r="C198" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D198" s="6">
+        <v>3</v>
+      </c>
+      <c r="E198" s="6">
+        <v>3</v>
+      </c>
+      <c r="F198" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G198" s="6">
+        <v>10</v>
+      </c>
+      <c r="H198" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="199" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B199" s="5">
+        <v>195</v>
+      </c>
+      <c r="C199" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D199" s="6">
+        <v>3</v>
+      </c>
+      <c r="E199" s="6">
+        <v>3</v>
+      </c>
+      <c r="F199" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G199" s="6">
+        <v>10</v>
+      </c>
+      <c r="H199" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B200" s="5">
+        <v>196</v>
+      </c>
+      <c r="C200" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D200" s="6">
+        <v>3</v>
+      </c>
+      <c r="E200" s="6">
+        <v>3</v>
+      </c>
+      <c r="F200" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G200" s="6">
+        <v>10</v>
+      </c>
+      <c r="H200" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="201" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B201" s="5">
+        <v>197</v>
+      </c>
+      <c r="C201" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D201" s="6">
+        <v>3</v>
+      </c>
+      <c r="E201" s="6">
+        <v>3</v>
+      </c>
+      <c r="F201" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G201" s="6">
+        <v>10</v>
+      </c>
+      <c r="H201" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="202" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B202" s="5">
+        <v>198</v>
+      </c>
+      <c r="C202" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D202" s="6">
+        <v>3</v>
+      </c>
+      <c r="E202" s="6">
+        <v>3</v>
+      </c>
+      <c r="F202" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G202" s="6">
+        <v>10</v>
+      </c>
+      <c r="H202" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="203" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B203" s="5">
+        <v>199</v>
+      </c>
+      <c r="C203" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D203" s="6">
+        <v>3</v>
+      </c>
+      <c r="E203" s="6">
+        <v>3</v>
+      </c>
+      <c r="F203" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G203" s="6">
+        <v>10</v>
+      </c>
+      <c r="H203" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="204" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B204" s="5">
+        <v>200</v>
+      </c>
+      <c r="C204" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D204" s="6">
+        <v>3</v>
+      </c>
+      <c r="E204" s="6">
+        <v>3</v>
+      </c>
+      <c r="F204" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G204" s="6">
+        <v>10</v>
+      </c>
+      <c r="H204" s="6">
         <v>20</v>
       </c>
     </row>
@@ -1861,10 +5359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC1586B-6A73-4ED9-BBD3-EF79BC3A505F}">
-  <dimension ref="A2:F6"/>
+  <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1963,6 +5461,108 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
+        <v>51</v>
+      </c>
+      <c r="D7" s="6">
+        <v>75</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6">
+        <v>76</v>
+      </c>
+      <c r="D8" s="6">
+        <v>100</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>101</v>
+      </c>
+      <c r="D9" s="6">
+        <v>125</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6">
+        <v>126</v>
+      </c>
+      <c r="D10" s="6">
+        <v>150</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6">
+        <v>151</v>
+      </c>
+      <c r="D11" s="6">
+        <v>175</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
+        <v>176</v>
+      </c>
+      <c r="D12" s="6">
+        <v>200</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>